<commit_message>
Improved labeling of cells (Delta t) :-)
</commit_message>
<xml_diff>
--- a/doc/spreadsheets/EstimationOfMarginBufferAndPenalty.xlsx
+++ b/doc/spreadsheets/EstimationOfMarginBufferAndPenalty.xlsx
@@ -1,34 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Dropbox/Paper 2018 Smart Contracts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath-smart-derivative-contract/doc/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68E31B5-705A-5A4C-B627-424BBEF17FCF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9228AE73-5AAB-7044-A24E-DD7A7A5FA81A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19900" xr2:uid="{EF3ED18B-4C31-EA44-907F-3049561214C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
-  <si>
-    <t>sqrt(T)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>T</t>
   </si>
@@ -247,6 +252,12 @@
   </si>
   <si>
     <t>Christian Fries, Peter Kohl-Landgraf</t>
+  </si>
+  <si>
+    <t>∆t</t>
+  </si>
+  <si>
+    <t>sqrt(∆t)</t>
   </si>
 </sst>
 </file>
@@ -255,8 +266,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -412,7 +423,7 @@
     <xf numFmtId="11" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -422,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -458,10 +469,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,9 +486,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,7 +504,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -792,7 +803,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,48 +820,48 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4">
         <f>1/250</f>
@@ -860,10 +871,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D8" s="4">
         <f>SQRT(D7)</f>
@@ -873,10 +884,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5">
         <f>D6*D8</f>
@@ -884,7 +895,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -892,22 +903,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="21">
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -918,10 +929,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4">
         <v>365</v>
@@ -930,23 +941,23 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D15" s="12">
         <v>1E-4</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="4">
         <f>1-D15</f>
@@ -956,10 +967,10 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D17" s="4">
         <f>POWER(D16,1/D14)</f>
@@ -969,10 +980,10 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D18" s="6">
         <f>1-D17</f>
@@ -984,7 +995,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
@@ -992,10 +1003,10 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D20" s="26">
         <f>NORMINV(D18,0,$D$12)</f>
@@ -1003,30 +1014,30 @@
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D21" s="4">
         <v>10</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D22" s="7">
         <f>D21*D20</f>
@@ -1034,12 +1045,12 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="6"/>
@@ -1047,10 +1058,10 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D24" s="29">
         <f>I31</f>
@@ -1058,15 +1069,15 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="7">
         <f>D22-D24*D21</f>
@@ -1075,66 +1086,66 @@
       <c r="E25" s="3"/>
       <c r="F25" s="13"/>
       <c r="H25" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
       <c r="H26" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="19">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D27" s="24">
         <v>0.03</v>
       </c>
       <c r="E27" s="3"/>
       <c r="H27" s="18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="22">
         <v>14</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D28" s="32">
         <f>D27*D25*100*100</f>
         <v>-10.806916885802128</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I28" s="18">
         <f>I26*SQRT(I27)</f>
@@ -1143,10 +1154,10 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I29" s="20">
         <v>0</v>
@@ -1154,7 +1165,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H30" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I30" s="18">
         <f>(0-I29)/I28</f>
@@ -1163,10 +1174,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I31" s="30">
         <f>(0-I29)*_xlfn.NORM.DIST(I30,0,1,TRUE)+I28*_xlfn.NORM.DIST(I30,0,1,FALSE)</f>
@@ -1175,19 +1186,19 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="31">
         <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="26">
@@ -1198,7 +1209,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="7">
@@ -1207,38 +1218,38 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D35" s="32">
         <f>D34*D27*100*100</f>
         <v>-15.300000000000002</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="7">
         <v>0.01</v>
@@ -1247,10 +1258,10 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="7">
         <f>NORMINV(D38,0,1)</f>
@@ -1260,10 +1271,10 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" s="7">
         <f>D33/D39</f>
@@ -1273,10 +1284,10 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41" s="2">
         <f>D40/SQRT(14)</f>
@@ -1284,7 +1295,7 @@
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>